<commit_message>
Added an electrode location column to the main dataframe and implemented sorting of the electrode locations from A1-O15. Still doesn't work on Sample 8B for 5hz however, not sure why
</commit_message>
<xml_diff>
--- a/PE loop Sample 8/Sample A_monopolar/Unnormalized_Pmax_Sample_8A_100kHz.xlsx
+++ b/PE loop Sample 8/Sample A_monopolar/Unnormalized_Pmax_Sample_8A_100kHz.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,165 +444,250 @@
           <t>Unnormalized P_max</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Electrode Locations</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A11_monopolar_10V_100kHz.txt</t>
+          <t>A2_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12.495424</v>
+        <v>10.764196</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A14_monopolar_10V_100kHz.txt</t>
+          <t>A3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14.175679</v>
+        <v>11.146486</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A2_monopolar_10V_100kHz.txt</t>
+          <t>A8_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.764196</v>
+        <v>11.239328</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A8</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A3_monopolar_10V_100kHz.txt</t>
+          <t>A9_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.146486</v>
+        <v>11.845531</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A9</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A8_monopolar_10V_100kHz.txt</t>
+          <t>A11_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.239328</v>
+        <v>12.495424</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A11</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A9_monopolar_10V_100kHz.txt</t>
+          <t>A14_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11.845531</v>
+        <v>14.175679</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A14</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>B13_monopolar_10V_100kHz.txt</t>
+          <t>B6_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>13.857104</v>
+        <v>12.81764</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>B6</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>B15_monopolar_10V_100kHz.txt</t>
+          <t>B13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>14.117426</v>
+        <v>13.857104</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>B13</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>B6_monopolar_10V_100kHz.txt</t>
+          <t>B15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12.81764</v>
+        <v>14.117426</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>B15</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C11_monopolar_10V_100kHz.txt</t>
+          <t>C1_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>13.396536</v>
+        <v>11.166511</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C13_monopolar_10V_100kHz.txt</t>
+          <t>C5_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12.870432</v>
+        <v>12.497244</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>C5</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C15_monopolar_10V_100kHz.txt</t>
+          <t>C7_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>13.312796</v>
+        <v>13.037911</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C1_monopolar_10V_100kHz.txt</t>
+          <t>C9_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11.166511</v>
+        <v>13.056116</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>C9</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C5_monopolar_10V_100kHz.txt</t>
+          <t>C11_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12.497244</v>
+        <v>13.396536</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>C11</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C7_monopolar_10V_100kHz.txt</t>
+          <t>C13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13.037911</v>
+        <v>12.870432</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>C13</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C9_monopolar_10V_100kHz.txt</t>
+          <t>C15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13.056116</v>
+        <v>13.312796</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>C15</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -614,65 +699,100 @@
       <c r="B18" t="n">
         <v>10.658611</v>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E10_monopolar_10V_100kHz.txt</t>
+          <t>E1_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>12.895918</v>
+        <v>11.747227</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>E1</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E12_monopolar_10V_100kHz.txt</t>
+          <t>E4_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>13.777006</v>
+        <v>11.326708</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>E4</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>E1_monopolar_10V_100kHz.txt</t>
+          <t>E5_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11.747227</v>
+        <v>12.398941</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>E5</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E4_monopolar_10V_100kHz.txt</t>
+          <t>E8_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>11.326708</v>
+        <v>12.677466</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>E8</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E5_monopolar_10V_100kHz.txt</t>
+          <t>E10_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12.398941</v>
+        <v>12.895918</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>E10</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>E8_monopolar_10V_100kHz.txt</t>
+          <t>E12_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>12.677466</v>
+        <v>13.777006</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>E12</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -684,6 +804,11 @@
       <c r="B25" t="n">
         <v>13.403818</v>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>F14</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -694,95 +819,145 @@
       <c r="B26" t="n">
         <v>13.587681</v>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>F15</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>G10_monopolar_10V_100kHz.txt</t>
+          <t>G2_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>13.975432</v>
+        <v>12.850407</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>G2</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>G11_monopolar_10V_100kHz.txt</t>
+          <t>G3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>13.733315</v>
+        <v>12.180489</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>G3</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>G13_monopolar_10V_100kHz.txt</t>
+          <t>G5_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>13.79703</v>
+        <v>13.356486</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>G5</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>G15_monopolar_10V_100kHz.txt</t>
+          <t>G7_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>14.104683</v>
+        <v>13.873488</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>G7</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>G2_monopolar_10V_100kHz.txt</t>
+          <t>G9_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>12.850407</v>
+        <v>13.731495</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>G9</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>G3_monopolar_10V_100kHz.txt</t>
+          <t>G10_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>12.180489</v>
+        <v>13.975432</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>G10</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>G5_monopolar_10V_100kHz.txt</t>
+          <t>G11_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>13.356486</v>
+        <v>13.733315</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>G11</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>G7_monopolar_10V_100kHz.txt</t>
+          <t>G13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>13.873488</v>
+        <v>13.79703</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>G13</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>G9_monopolar_10V_100kHz.txt</t>
+          <t>G15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>13.731495</v>
+        <v>14.104683</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>G15</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -794,75 +969,115 @@
       <c r="B36" t="n">
         <v>14.441462</v>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>H9</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>I10_monopolar_10V_100kHz.txt</t>
+          <t>I1_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>15.615639</v>
+        <v>13.784287</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>I1</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>I11_monopolar_10V_100kHz.txt</t>
+          <t>I3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>16.234584</v>
+        <v>14.832854</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>I3</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>I15_monopolar_10V_100kHz.txt</t>
+          <t>I6_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>15.821347</v>
+        <v>15.156891</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>I6</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>I1_monopolar_10V_100kHz.txt</t>
+          <t>I8_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>13.784287</v>
+        <v>15.666611</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>I8</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>I3_monopolar_10V_100kHz.txt</t>
+          <t>I10_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>14.832854</v>
+        <v>15.615639</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>I10</t>
+        </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>I6_monopolar_10V_100kHz.txt</t>
+          <t>I11_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>15.156891</v>
+        <v>16.234584</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>I11</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>I8_monopolar_10V_100kHz.txt</t>
+          <t>I15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>15.666611</v>
+        <v>15.821347</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>I15</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -874,255 +1089,385 @@
       <c r="B44" t="n">
         <v>17.332303</v>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>J13</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>K11_monopolar_10V_100kHz.txt</t>
+          <t>K2_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>19.494973</v>
+        <v>16.620515</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>K2</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>K13_monopolar_10V_100kHz.txt</t>
+          <t>K3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>18.602962</v>
+        <v>17.010087</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>K3</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>K2_monopolar_10V_100kHz.txt</t>
+          <t>K6_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>16.620515</v>
+        <v>18.240697</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>K6</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>K3_monopolar_10V_100kHz.txt</t>
+          <t>K9_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>17.010087</v>
+        <v>18.655755</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>K9</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>K6_monopolar_10V_100kHz.txt</t>
+          <t>K11_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>18.240697</v>
+        <v>19.494973</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>K11</t>
+        </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>K9_monopolar_10V_100kHz.txt</t>
+          <t>K13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>18.655755</v>
+        <v>18.602962</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>K13</t>
+        </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>L15_monopolar_10V_100kHz.txt</t>
+          <t>L7_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>21.81966</v>
+        <v>21.064182</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>L7</t>
+        </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>L7_monopolar_10V_100kHz.txt</t>
+          <t>L8_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>21.064182</v>
+        <v>21.661283</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>L8</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>L8_monopolar_10V_100kHz.txt</t>
+          <t>L15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>21.661283</v>
+        <v>21.81966</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>L15</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>M12_monopolar_10V_100kHz.txt</t>
+          <t>M3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>22.547832</v>
+        <v>18.473712</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>M13_monopolar_10V_100kHz.txt</t>
+          <t>M5_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>22.899174</v>
+        <v>21.781431</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>M5</t>
+        </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>M15_monopolar_10V_100kHz.txt</t>
+          <t>M12_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>24.362799</v>
+        <v>22.547832</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>M12</t>
+        </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>M3_monopolar_10V_100kHz.txt</t>
+          <t>M13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>18.473712</v>
+        <v>22.899174</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>M13</t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>M5_monopolar_10V_100kHz.txt</t>
+          <t>M15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>21.781431</v>
+        <v>24.362799</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>M15</t>
+        </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>N10_monopolar_10V_100kHz.txt</t>
+          <t>N1_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>24.939875</v>
+        <v>16.940911</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>N1</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>N1_monopolar_10V_100kHz.txt</t>
+          <t>N8_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>16.940911</v>
+        <v>24.417412</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>N8</t>
+        </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>N8_monopolar_10V_100kHz.txt</t>
+          <t>N10_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>24.417412</v>
+        <v>24.939875</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>N10</t>
+        </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>O12_monopolar_10V_100kHz.txt</t>
+          <t>O1_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>20.434314</v>
+        <v>14.208447</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>O1</t>
+        </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>O13_monopolar_10V_100kHz.txt</t>
+          <t>O3_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>19.766216</v>
+        <v>22.706209</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>O3</t>
+        </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>O15_monopolar_10V_100kHz.txt</t>
+          <t>O5_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>16.074387</v>
+        <v>25.780913</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>O5</t>
+        </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>O1_monopolar_10V_100kHz.txt</t>
+          <t>O7_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>14.208447</v>
+        <v>25.826424</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>O7</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>O3_monopolar_10V_100kHz.txt</t>
+          <t>O9_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>22.706209</v>
+        <v>24.337313</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>O9</t>
+        </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>O5_monopolar_10V_100kHz.txt</t>
+          <t>O12_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>25.780913</v>
+        <v>20.434314</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>O12</t>
+        </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>O7_monopolar_10V_100kHz.txt</t>
+          <t>O13_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>25.826424</v>
+        <v>19.766216</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>O13</t>
+        </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>O9_monopolar_10V_100kHz.txt</t>
+          <t>O15_monopolar_10V_100kHz.txt</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>24.337313</v>
+        <v>16.074387</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>O15</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>